<commit_message>
Finished up testing documentation for Planetarium version 1.0
</commit_message>
<xml_diff>
--- a/Planetarium Requirements Documentation.xlsx
+++ b/Planetarium Requirements Documentation.xlsx
@@ -572,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -630,19 +630,13 @@
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1532,10 +1526,10 @@
       <c r="B4" s="19">
         <v>45584.0</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>45589.0</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1543,13 +1537,13 @@
       <c r="A5" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>45590.0</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <v>45591.0</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1557,10 +1551,10 @@
       <c r="A6" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>45591.0</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <v>45593.0</v>
       </c>
     </row>
@@ -1568,10 +1562,10 @@
       <c r="A7" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="15">
         <v>45594.0</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="15">
         <v>45597.0</v>
       </c>
     </row>
@@ -1582,7 +1576,7 @@
       <c r="B9" s="15">
         <v>45580.0</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="15">
         <v>45597.0</v>
       </c>
     </row>

</xml_diff>